<commit_message>
신동훈 Enum TowerName 추가
</commit_message>
<xml_diff>
--- a/Design/DataTable/Enums.xlsx
+++ b/Design/DataTable/Enums.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ComputerScience\Project\PlumTowerDefence\PlumTowerDefecne\Design\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\신동훈\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75387801-B2C8-4A44-89D7-6B89519656D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7557951A-B5CC-4753-BE9D-9307D08F10E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="1215" windowWidth="23880" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="146">
   <si>
     <t>이 파일은 CSV파일로 저장하지 마세요!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -534,6 +534,78 @@
   </si>
   <si>
     <t>수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnumName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Typename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TypeValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TowerName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hourglass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poison</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackBuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpeedBuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Laser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Missile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electric</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gatling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cannon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09.03 23:13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신동훈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1039,6 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,7 +1130,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
@@ -1339,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1356,22 +1428,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -1662,16 +1734,16 @@
       <c r="C16" s="20">
         <v>7</v>
       </c>
-      <c r="I16" s="46" t="s">
+      <c r="I16" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="46" t="s">
+      <c r="J16" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="46" t="s">
+      <c r="K16" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="L16" s="40" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1683,16 +1755,16 @@
       <c r="C17" s="20">
         <v>8</v>
       </c>
-      <c r="I17" s="46" t="s">
+      <c r="I17" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J17" s="46" t="s">
+      <c r="J17" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="46" t="s">
+      <c r="K17" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="46" t="s">
+      <c r="L17" s="40" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1704,16 +1776,16 @@
       <c r="C18" s="20">
         <v>9</v>
       </c>
-      <c r="I18" s="46" t="s">
+      <c r="I18" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J18" s="46" t="s">
+      <c r="J18" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="K18" s="46" t="s">
+      <c r="K18" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="L18" s="46" t="s">
+      <c r="L18" s="40" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1725,16 +1797,16 @@
       <c r="C19" s="20">
         <v>10</v>
       </c>
-      <c r="I19" s="46" t="s">
+      <c r="I19" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="46" t="s">
+      <c r="J19" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="L19" s="46" t="s">
+      <c r="L19" s="40" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1746,16 +1818,16 @@
       <c r="C20" s="20">
         <v>11</v>
       </c>
-      <c r="I20" s="46" t="s">
+      <c r="I20" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="J20" s="46" t="s">
+      <c r="J20" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="K20" s="46" t="s">
+      <c r="K20" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="L20" s="46" t="s">
+      <c r="L20" s="40" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1767,16 +1839,16 @@
       <c r="C21" s="20">
         <v>12</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J21" s="46" t="s">
+      <c r="J21" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="K21" s="46" t="s">
+      <c r="K21" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="40" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1788,16 +1860,16 @@
       <c r="C22" s="20">
         <v>13</v>
       </c>
-      <c r="I22" s="46" t="s">
+      <c r="I22" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="J22" s="46" t="s">
+      <c r="J22" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="K22" s="46" t="s">
+      <c r="K22" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="L22" s="46" t="s">
+      <c r="L22" s="40" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1809,58 +1881,58 @@
       <c r="C23" s="23">
         <v>14</v>
       </c>
-      <c r="I23" s="46" t="s">
+      <c r="I23" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="46" t="s">
+      <c r="J23" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="K23" s="46" t="s">
+      <c r="K23" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="40" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J24" s="46" t="s">
+      <c r="J24" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="K24" s="46" t="s">
+      <c r="K24" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="40" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I25" s="46" t="s">
+      <c r="I25" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="J25" s="46" t="s">
+      <c r="J25" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="K25" s="46" t="s">
+      <c r="K25" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="L25" s="46" t="s">
+      <c r="L25" s="40" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="J26" s="46" t="s">
+      <c r="J26" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="K26" s="46" t="s">
+      <c r="K26" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="L26" s="46" t="s">
+      <c r="L26" s="40" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1874,16 +1946,16 @@
       <c r="C27" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="J27" s="46" t="s">
+      <c r="J27" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="K27" s="46" t="s">
+      <c r="K27" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="L27" s="46" t="s">
+      <c r="L27" s="40" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1896,6 +1968,18 @@
       </c>
       <c r="C28" s="20">
         <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" t="s">
+        <v>131</v>
+      </c>
+      <c r="L28" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -2311,6 +2395,119 @@
       </c>
       <c r="C88" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B91" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C91" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="18"/>
+      <c r="B92" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C92" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="18"/>
+      <c r="B93" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C93" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="18"/>
+      <c r="B94" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C94" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="18"/>
+      <c r="B95" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="18"/>
+      <c r="B96" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C96" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="18"/>
+      <c r="B97" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C97" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="18"/>
+      <c r="B98" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C98" s="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="18"/>
+      <c r="B99" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C99" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="18"/>
+      <c r="B100" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C100" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="21"/>
+      <c r="B101" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C101" s="23">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
신동훈 Enum TowerName 수정
</commit_message>
<xml_diff>
--- a/Design/DataTable/Enums.xlsx
+++ b/Design/DataTable/Enums.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\신동훈\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7557951A-B5CC-4753-BE9D-9307D08F10E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BCA971-FA56-4281-8EE7-DEB6AF6158FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="1215" windowWidth="23880" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="2175" windowWidth="23880" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="153">
   <si>
     <t>이 파일은 CSV파일로 저장하지 마세요!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -606,6 +606,34 @@
   </si>
   <si>
     <t>추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09.03 13:13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신동훈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TowerName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mine</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1040,7 +1068,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1130,6 +1158,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="나쁨" xfId="1" builtinId="27"/>
@@ -1411,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28:L28"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1990,6 +2020,18 @@
       <c r="C29" s="20">
         <v>2</v>
       </c>
+      <c r="I29" t="s">
+        <v>148</v>
+      </c>
+      <c r="J29" t="s">
+        <v>149</v>
+      </c>
+      <c r="K29" t="s">
+        <v>150</v>
+      </c>
+      <c r="L29" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
@@ -2501,13 +2543,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="21"/>
-      <c r="B101" s="36" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="18"/>
+      <c r="B101" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C101" s="23">
+      <c r="C101" s="20">
         <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B102" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C102" s="47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B103" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C103" s="47">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="22"/>
+      <c r="B104" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C104" s="48">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
김다희 Enum에 PickaxeType 추가
</commit_message>
<xml_diff>
--- a/Design/DataTable/Enums.xlsx
+++ b/Design/DataTable/Enums.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ComputerScience\Project\PlumTowerDefence\PlumTowerDefecne\Design\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdhhi\Desktop\서울과학기술대학교\PLUM\2022 8월 게임 프로젝트\Copy\PlumTowerDefecne\Design\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078A99AB-7C2D-4417-A96D-124806FDCAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462814A5-6827-4EC5-A4E6-A6D8FA92FDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5628" yWindow="1176" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="163">
   <si>
     <t>이 파일은 CSV파일로 저장하지 마세요!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -650,6 +650,30 @@
   </si>
   <si>
     <t>수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PickaxeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09.04 21:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1458,23 +1482,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L30" sqref="I27:L30"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.75" customWidth="1"/>
-    <col min="10" max="10" width="9.875" customWidth="1"/>
-    <col min="11" max="11" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.69921875" customWidth="1"/>
+    <col min="10" max="10" width="9.8984375" customWidth="1"/>
+    <col min="11" max="11" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1516,7 @@
       <c r="K1" s="48"/>
       <c r="L1" s="49"/>
     </row>
-    <row r="2" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1515,7 +1539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1538,7 +1562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="12"/>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -1559,7 +1583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -1580,7 +1604,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="I6" s="26" t="s">
         <v>40</v>
       </c>
@@ -1594,7 +1618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="I7" s="26" t="s">
         <v>48</v>
       </c>
@@ -1608,7 +1632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I8" s="26" t="s">
         <v>49</v>
       </c>
@@ -1622,7 +1646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1669,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1692,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
         <v>18</v>
@@ -1689,7 +1713,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>19</v>
@@ -1710,7 +1734,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
         <v>20</v>
@@ -1731,7 +1755,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
         <v>21</v>
@@ -1752,7 +1776,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="18"/>
       <c r="B15" s="19" t="s">
         <v>22</v>
@@ -1773,7 +1797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
         <v>23</v>
@@ -1794,7 +1818,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
         <v>24</v>
@@ -1815,7 +1839,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="18"/>
       <c r="B18" s="19" t="s">
         <v>25</v>
@@ -1836,7 +1860,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="18"/>
       <c r="B19" s="19" t="s">
         <v>26</v>
@@ -1857,7 +1881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="18"/>
       <c r="B20" s="19" t="s">
         <v>27</v>
@@ -1878,7 +1902,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="18"/>
       <c r="B21" s="19" t="s">
         <v>28</v>
@@ -1899,7 +1923,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="18"/>
       <c r="B22" s="19" t="s">
         <v>29</v>
@@ -1920,7 +1944,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="21"/>
       <c r="B23" s="22" t="s">
         <v>30</v>
@@ -1941,7 +1965,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="I24" s="40" t="s">
         <v>106</v>
       </c>
@@ -1955,7 +1979,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="I25" s="40" t="s">
         <v>114</v>
       </c>
@@ -1969,7 +1993,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I26" s="40" t="s">
         <v>123</v>
       </c>
@@ -1983,7 +2007,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="15" t="s">
         <v>1</v>
       </c>
@@ -2006,7 +2030,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="18" t="s">
         <v>41</v>
       </c>
@@ -2029,7 +2053,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="18"/>
       <c r="B29" s="24" t="s">
         <v>36</v>
@@ -2050,7 +2074,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" s="18"/>
       <c r="B30" s="24" t="s">
         <v>37</v>
@@ -2071,7 +2095,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="21"/>
       <c r="B31" s="25" t="s">
         <v>38</v>
@@ -2079,9 +2103,21 @@
       <c r="C31" s="23">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I31" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="J31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="L31" s="40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="15" t="s">
         <v>1</v>
       </c>
@@ -2092,7 +2128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>43</v>
       </c>
@@ -2103,7 +2139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="18"/>
       <c r="B37" s="24" t="s">
         <v>45</v>
@@ -2112,7 +2148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="18"/>
       <c r="B38" s="24" t="s">
         <v>46</v>
@@ -2121,7 +2157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="21"/>
       <c r="B39" s="25" t="s">
         <v>47</v>
@@ -2130,8 +2166,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" s="27" t="s">
         <v>52</v>
       </c>
@@ -2142,7 +2178,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" s="30" t="s">
         <v>53</v>
       </c>
@@ -2153,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" s="30"/>
       <c r="B45" s="24" t="s">
         <v>55</v>
@@ -2162,7 +2198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" s="30"/>
       <c r="B46" s="24" t="s">
         <v>56</v>
@@ -2171,7 +2207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" s="30"/>
       <c r="B47" s="24" t="s">
         <v>57</v>
@@ -2180,7 +2216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="30"/>
       <c r="B48" s="24" t="s">
         <v>92</v>
@@ -2189,7 +2225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" s="30"/>
       <c r="B49" s="24" t="s">
         <v>93</v>
@@ -2198,7 +2234,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A50" s="32"/>
       <c r="B50" s="25" t="s">
         <v>94</v>
@@ -2207,8 +2243,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" s="27" t="s">
         <v>52</v>
       </c>
@@ -2219,7 +2255,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" s="30" t="s">
         <v>69</v>
       </c>
@@ -2230,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
         <v>83</v>
       </c>
@@ -2238,7 +2274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="30"/>
       <c r="B57" s="24" t="s">
         <v>75</v>
@@ -2247,7 +2283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="30"/>
       <c r="B58" s="24" t="s">
         <v>76</v>
@@ -2256,7 +2292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="30"/>
       <c r="B59" s="24" t="s">
         <v>77</v>
@@ -2265,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A60" s="21"/>
       <c r="B60" s="36" t="s">
         <v>78</v>
@@ -2274,8 +2310,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="27" t="s">
         <v>52</v>
       </c>
@@ -2286,7 +2322,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A65" s="30" t="s">
         <v>70</v>
       </c>
@@ -2297,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66" s="30"/>
       <c r="B66" s="24" t="s">
         <v>71</v>
@@ -2306,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67" s="30"/>
       <c r="B67" s="24" t="s">
         <v>72</v>
@@ -2315,7 +2351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A68" s="32"/>
       <c r="B68" s="25" t="s">
         <v>73</v>
@@ -2324,8 +2360,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" s="15" t="s">
         <v>86</v>
       </c>
@@ -2336,7 +2372,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71" s="18" t="s">
         <v>87</v>
       </c>
@@ -2347,7 +2383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" s="18"/>
       <c r="B72" s="34" t="s">
         <v>113</v>
@@ -2356,7 +2392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A73" s="18"/>
       <c r="B73" s="34" t="s">
         <v>102</v>
@@ -2365,12 +2401,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" s="16"/>
       <c r="B74" s="38"/>
       <c r="C74" s="38"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>1</v>
       </c>
@@ -2381,7 +2417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>99</v>
       </c>
@@ -2392,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A79" s="1"/>
       <c r="B79" s="39" t="s">
         <v>119</v>
@@ -2401,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" s="1"/>
       <c r="B80" s="39" t="s">
         <v>100</v>
@@ -2410,7 +2446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" s="1"/>
       <c r="B81" s="39" t="s">
         <v>101</v>
@@ -2419,7 +2455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A82" s="1"/>
       <c r="B82" s="39" t="s">
         <v>102</v>
@@ -2428,7 +2464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" s="1"/>
       <c r="B83" s="39" t="s">
         <v>152</v>
@@ -2437,7 +2473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>1</v>
       </c>
@@ -2448,7 +2484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>111</v>
       </c>
@@ -2459,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" s="1"/>
       <c r="B88" s="39" t="s">
         <v>104</v>
@@ -2468,7 +2504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" s="1"/>
       <c r="B89" s="39" t="s">
         <v>105</v>
@@ -2477,8 +2513,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" s="15" t="s">
         <v>128</v>
       </c>
@@ -2489,7 +2525,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" s="18" t="s">
         <v>131</v>
       </c>
@@ -2500,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" s="18"/>
       <c r="B93" s="34" t="s">
         <v>133</v>
@@ -2509,7 +2545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" s="18"/>
       <c r="B94" s="34" t="s">
         <v>134</v>
@@ -2518,7 +2554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" s="18"/>
       <c r="B95" s="34" t="s">
         <v>135</v>
@@ -2527,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" s="18"/>
       <c r="B96" s="34" t="s">
         <v>136</v>
@@ -2536,7 +2572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="18"/>
       <c r="B97" s="34" t="s">
         <v>137</v>
@@ -2545,7 +2581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="18"/>
       <c r="B98" s="34" t="s">
         <v>138</v>
@@ -2554,7 +2590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" s="18"/>
       <c r="B99" s="34" t="s">
         <v>139</v>
@@ -2563,7 +2599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" s="18"/>
       <c r="B100" s="34" t="s">
         <v>140</v>
@@ -2572,7 +2608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A101" s="18"/>
       <c r="B101" s="34" t="s">
         <v>141</v>
@@ -2581,7 +2617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A102" s="18"/>
       <c r="B102" s="34" t="s">
         <v>142</v>
@@ -2590,7 +2626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B103" s="34" t="s">
         <v>151</v>
       </c>
@@ -2598,7 +2634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B104" s="34" t="s">
         <v>146</v>
       </c>
@@ -2606,13 +2642,63 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A105" s="22"/>
       <c r="B105" s="36" t="s">
         <v>147</v>
       </c>
       <c r="C105" s="42">
         <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A109" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A110" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C110" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A111" s="18"/>
+      <c r="B111" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C111" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A112" s="18"/>
+      <c r="B112" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C112" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A113" s="21"/>
+      <c r="B113" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C113" s="23">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
강민재 enum LaneBuffType 추가
</commit_message>
<xml_diff>
--- a/Design/DataTable/Enums.xlsx
+++ b/Design/DataTable/Enums.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\강민재\Documents\GitHub\PlumTowerDefecne\PlumTowerDefecne\Design\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC2B651-3D62-4642-BE4A-0B5F601D1E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF11CB65-D9AC-4D40-8BD3-37140FF48811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="209">
   <si>
     <t>이 파일은 CSV파일로 저장하지 마세요!!</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -714,6 +714,142 @@
   </si>
   <si>
     <t>09.05 15:43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강민재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnumName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Typename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TypeValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaneBuffType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllHealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllDealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllHealShield</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllDealShield</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllBuffArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AllNurfArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaterHealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroundHealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>FireHealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElectricHealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaterDealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroundDealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElectricDealHp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaterBuffArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroundBuffArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>FireBuffArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElectricBuffArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaterNurfArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>GroundNurfArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>FireNurfArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElectricNurfArmor</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ArrowBuff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlowBuff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PoisonBuff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>FlameBuff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>LazerBuff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MissileBuff</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>09.06 13:49</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1530,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L120"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2178,8 +2314,22 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="I33" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="K33" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="L33" s="40" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A35" s="15" t="s">
         <v>1</v>
       </c>
@@ -2190,7 +2340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>43</v>
       </c>
@@ -2201,7 +2351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A37" s="18"/>
       <c r="B37" s="24" t="s">
         <v>45</v>
@@ -2210,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A38" s="18"/>
       <c r="B38" s="24" t="s">
         <v>46</v>
@@ -2219,7 +2369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="21"/>
       <c r="B39" s="25" t="s">
         <v>47</v>
@@ -2228,8 +2378,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A43" s="27" t="s">
         <v>52</v>
       </c>
@@ -2240,7 +2390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A44" s="30" t="s">
         <v>53</v>
       </c>
@@ -2251,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A45" s="30"/>
       <c r="B45" s="24" t="s">
         <v>55</v>
@@ -2260,7 +2410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A46" s="30"/>
       <c r="B46" s="24" t="s">
         <v>56</v>
@@ -2269,7 +2419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A47" s="30"/>
       <c r="B47" s="24" t="s">
         <v>57</v>
@@ -2278,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A48" s="30"/>
       <c r="B48" s="24" t="s">
         <v>92</v>
@@ -2819,6 +2969,271 @@
       </c>
       <c r="C120" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A123" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A124" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B124" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A125" s="1"/>
+      <c r="B125" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C125" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A126" s="1"/>
+      <c r="B126" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="C126" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A127" s="1"/>
+      <c r="B127" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C127" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A128" s="1"/>
+      <c r="B128" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="C128" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A129" s="1"/>
+      <c r="B129" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="C129" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A130" s="1"/>
+      <c r="B130" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="C130" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A131" s="1"/>
+      <c r="B131" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C131" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A132" s="1"/>
+      <c r="B132" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C132" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A133" s="1"/>
+      <c r="B133" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C133" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A134" s="1"/>
+      <c r="B134" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C134" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A135" s="1"/>
+      <c r="B135" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="C135" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A136" s="1"/>
+      <c r="B136" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="C136" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A137" s="1"/>
+      <c r="B137" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="C137" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A138" s="1"/>
+      <c r="B138" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="C138" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A139" s="1"/>
+      <c r="B139" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="C139" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A140" s="1"/>
+      <c r="B140" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="C140" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A141" s="1"/>
+      <c r="B141" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="C141" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A142" s="1"/>
+      <c r="B142" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="C142" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A143" s="1"/>
+      <c r="B143" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="C143" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A144" s="1"/>
+      <c r="B144" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="C144" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A145" s="1"/>
+      <c r="B145" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="C145" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A146" s="1"/>
+      <c r="B146" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="C146" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A147" s="1"/>
+      <c r="B147" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="C147" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A148" s="1"/>
+      <c r="B148" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="C148" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A149" s="1"/>
+      <c r="B149" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="C149" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A150" s="1"/>
+      <c r="B150" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="C150" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A151" s="1"/>
+      <c r="B151" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="C151" s="1">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>